<commit_message>
requirements added for mapping challenges
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping.xlsx
+++ b/requirements/Requirements - conceptual mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/Documents/Conceptual-Mapping/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D200404D-A70C-2047-853A-52EEC19FEB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77608CAE-9E6F-4E4E-BCD5-03DC41699258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33180" yWindow="-900" windowWidth="34020" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Identifier</t>
   </si>
@@ -199,6 +199,27 @@
     <t>cm-r25</t>
   </si>
   <si>
+    <t>cm-r26</t>
+  </si>
+  <si>
+    <t>cm-r27</t>
+  </si>
+  <si>
+    <t>cm-r28</t>
+  </si>
+  <si>
+    <t>cm-r29</t>
+  </si>
+  <si>
+    <t>cm-r30</t>
+  </si>
+  <si>
+    <t>cm-r31</t>
+  </si>
+  <si>
+    <t>cm-r32</t>
+  </si>
+  <si>
     <t>A statement map can be linked to another statement map with none, one or several conditions</t>
   </si>
   <si>
@@ -206,6 +227,48 @@
   </si>
   <si>
     <t>A function may have nested functions</t>
+  </si>
+  <si>
+    <t>Datatype and language tags can be generated from one or more data sources</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C1 (KGC-WG)</t>
+  </si>
+  <si>
+    <t>A resource map can obtain data fields from different levels of iteration of the frame dat handles a data source</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C2a (KGC-WG)</t>
+  </si>
+  <si>
+    <t>A frame can have nested frames to access multi-value references</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C2b (KGC-WG)</t>
+  </si>
+  <si>
+    <t>A resource map can access multi-value references as lists or containers</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C3, C4 (KGC-WG)</t>
+  </si>
+  <si>
+    <t>Links between statements can happen without condition</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C5a (KGC-WG)</t>
+  </si>
+  <si>
+    <t>A statement map can have objects of type literal using data from different sources joining data sources in combined frames</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C5b (KGC-WG)</t>
+  </si>
+  <si>
+    <t>A statement map can have datatype and language tags using data from different sources joining data sources in combined frames</t>
+  </si>
+  <si>
+    <t>Mapping challenges - C5c (KGC-WG)</t>
   </si>
 </sst>
 </file>
@@ -636,7 +699,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -934,7 +997,7 @@
         <v>50</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C24" s="5"/>
       <c r="E24" s="12" t="s">
@@ -946,7 +1009,7 @@
         <v>51</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5"/>
       <c r="E25" s="12" t="s">
@@ -958,54 +1021,96 @@
         <v>52</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C26" s="5"/>
       <c r="E26" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13">
-      <c r="A27" s="13"/>
-      <c r="B27" s="4"/>
+    <row r="27" spans="1:5" ht="28">
+      <c r="A27" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="C27" s="9"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:5" ht="13">
-      <c r="A28" s="13"/>
-      <c r="B28" s="4"/>
+      <c r="E27" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="42">
+      <c r="A28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>65</v>
+      </c>
       <c r="C28" s="5"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:5" ht="13">
-      <c r="A29" s="13"/>
-      <c r="B29" s="12"/>
+      <c r="E28" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28">
+      <c r="A29" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="C29" s="5"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" ht="13">
-      <c r="A30" s="13"/>
-      <c r="B30" s="4"/>
+      <c r="E29" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28">
+      <c r="A30" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="C30" s="5"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:5" ht="13">
-      <c r="A31" s="13"/>
-      <c r="B31" s="4"/>
+      <c r="E30" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28">
+      <c r="A31" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="C31" s="5"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="1:5" ht="13">
-      <c r="A32" s="13"/>
-      <c r="B32" s="4"/>
+      <c r="E31" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="42">
+      <c r="A32" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="C32" s="5"/>
-      <c r="E32" s="12"/>
-    </row>
-    <row r="33" spans="1:5" ht="13">
-      <c r="A33" s="13"/>
-      <c r="B33" s="4"/>
+      <c r="E32" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="42">
+      <c r="A33" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="13">
       <c r="A34" s="13"/>

</xml_diff>

<commit_message>
minor details fixed and themis tests added
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping.xlsx
+++ b/requirements/Requirements - conceptual mapping.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/Documents/Conceptual-Mapping/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661DAC63-D581-0542-99A9-310583943C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9006F0-7601-B94D-A793-DB6242A7868F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="26940" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Themis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
   <si>
     <t>Identifier</t>
   </si>
@@ -121,9 +122,6 @@
     <t>A data source can specify the encoding</t>
   </si>
   <si>
-    <t>A source frame describes exacly one data source</t>
-  </si>
-  <si>
     <t>A mapping specifies statement maps to declare the transformation of frames into RDF triples</t>
   </si>
   <si>
@@ -143,12 +141,6 @@
   </si>
   <si>
     <t>A named graph can only be expressed as an IRI or blank node</t>
-  </si>
-  <si>
-    <t>A datatype tag can only be expressed as an IRI</t>
-  </si>
-  <si>
-    <t>A language tag can only be expressed as a Literal</t>
   </si>
   <si>
     <t>A statement map can describe constant and dynamic subjects, predicates, objects</t>
@@ -247,11 +239,6 @@
   </si>
   <si>
     <t>cm:DataAccessService dcat:servesDataset dcat:Dataset .</t>
-  </si>
-  <si>
-    <t>cm:StatementMap cm:hasFrame cm:CombinedFrame .
-cm:CombinedFrame cm:combinesFrame cm:SourceFrame, cm:CombinedFrame .
-cm:SourceFrame cm:hasDataSource cm:DataSource .</t>
   </si>
   <si>
     <t>cm:DataAccessService cm:hasProtocol skos:Concept . *</t>
@@ -281,12 +268,6 @@
     <t>cm:StatementMap cm:hasPredicate cm:ReferenceNodeMap .</t>
   </si>
   <si>
-    <t>cm:StatementMap cm:hasDatatype cm:ReferenceNodeMap .</t>
-  </si>
-  <si>
-    <t>cm:StatementMap cm:hasLanguage cm:LiteralMap .</t>
-  </si>
-  <si>
     <t>cm:StatementMap cm:hasSubject cm:NodeMap ;
     cm:hasPredicate cm:ReferenceNodeMap ;
     cm:hasObject cm:ResourceMap .
@@ -325,11 +306,6 @@
 (cm:Constant cm:DataField) rdfs:subClassOf cm:EvaluableExpression. *</t>
   </si>
   <si>
-    <t>cm:ConditionalStatementMap rdfs:subClassOf cm:StatementMap ;
-    cm:hasBooleanCondition cm:FunctionExpression .
-cm:FunctionExpression hasFunctionName skos:Concept .</t>
-  </si>
-  <si>
     <t>cm:ResourceMap cm:hasEvaluableExpression cm:FunctionExpression .
 cm:FunctionExpression cm:hasInput cm:ExpressionList .
 cm:ExpressionList rdfs:first cm:FunctionExpression ;
@@ -340,12 +316,6 @@
   </si>
   <si>
     <t>Comparison framework analysis and Mapping challenges - C3, C4 (KGC-WG)</t>
-  </si>
-  <si>
-    <t>cm:StatementMap cm:hasFrame cm:CombinedFrame ;
-    cm:hasObject cm:ResourceMap .
-cm:CombinedFrame cm:combinesFrame cm:SourceFrame, cm:CombinedFrame .
-cm:SourceFrame cm:hasDataSource cm:DataSource .</t>
   </si>
   <si>
     <t>cm:StatementMap cm:hasFrame cm:CombinedFrame ;
@@ -356,6 +326,200 @@
   </si>
   <si>
     <t>cm:DataSource cm:encoding xsd:string .</t>
+  </si>
+  <si>
+    <t>Themis test</t>
+  </si>
+  <si>
+    <t>SynchronousSource subclassof DataSource ;
+AsynchronousSource subclassof DataSource ;
+StreamSource subclassof DataSource ;</t>
+  </si>
+  <si>
+    <t>DataAccessService SubClassOf hasProtocol max 1 Concept ;</t>
+  </si>
+  <si>
+    <t>encoding domain DataSource ;</t>
+  </si>
+  <si>
+    <t>DataSource mediaType MediaType ;</t>
+  </si>
+  <si>
+    <t>DataAccessService hasSecurityScheme SecurityScheme ;</t>
+  </si>
+  <si>
+    <t>DataSource accessService DataAccessService ;</t>
+  </si>
+  <si>
+    <t>DataService servesDataset Dataset ;</t>
+  </si>
+  <si>
+    <t>StatementMap hasFrame CombinedFrame ;
+CombinedFrame SubClassOf combinesFrame exactly 2 Frame ;
+SourceFrame SubClassOf Frame ;
+SourceFrame hasDataSource DataSource ;
+SourceFrame hasNestedFrame SourceFrame ;</t>
+  </si>
+  <si>
+    <t>cm:StatementMap cm:hasFrame cm:CombinedFrame .
+cm:CombinedFrame cm:combinesFrame cm:SourceFrame, cm:CombinedFrame .
+cm:SourceFrame cm:hasDataSource cm:DataSource ;
+    cm:hasNestedFrame cm:SourceFrame .</t>
+  </si>
+  <si>
+    <t>A source frame describes exactly one data source</t>
+  </si>
+  <si>
+    <t>SourceFrame SubClassOf hasDataSource exactly 1 DataSource ;</t>
+  </si>
+  <si>
+    <t>StatementMap hasSubject NodeMap ;
+StatementMap hasPredicate ReferenceNodeMap ;
+StatementMap hasObject ResourceMap ;
+ReferenceNodeMap SubClassOf NodeMap ;
+NodeMap SubClassOf ResourceMap ;
+ResourceMap hasEvaluableExpression EvaluableExpression ;
+Constant SubClassOf EvaluableExpression ;
+DataField SubClassOf EvaluableExpression ;</t>
+  </si>
+  <si>
+    <t>StatementMap SubClassOf hasSubject exactly 1 NodeMap ;
+StatementMap SubClassOf hasPredicate exactly 1 ReferenceNodeMap ;
+StatementMap SubClassOf hasObject exactly 1 ResourceMap ;
+StatementMap SubClassOf hasNamedGraph max 1 NodeMap ;
+StatementMap SubClassOf hasDataType max 1 ReferenceNodeMap ;
+StatementMap SubClassOf hasLanguage max 1 LiteralMap ;</t>
+  </si>
+  <si>
+    <t>StatementMap SubClassOf hasNamedGraph max 1 NodeMap ;
+StatementMap SubClassOf hasDataType max 1 ReferenceNodeMap ;
+StatementMap SubClassOf hasLanguage max 1 LiteralMap ;
+ReferenceNodeMap SubClassOf NodeMap ;
+NodeMap SubClassOf ResourceMap ;
+LiteralMap SubClassOf ResourceMap ;
+ResourceMap hasEvaluableExpression EvaluableExpression ;
+Constant SubClassOf EvaluableExpression ;
+DataField SubClassOf EvaluableExpression ;</t>
+  </si>
+  <si>
+    <t>cm:StatementMap cm:hasFrame cm:CombinedFrame .
+cm:ResourceMap cm:hasEvaluableExpression cm:FunctionExpression .
+cm:FunctionExpression cm:hasInput cm:ExpressionList .
+cm:ExpressionList rdfs:first cm:DataField .
+cm:DataField cm:belongsToFrame cm:SourceFrame .
+cm:CombinedFrame cm:combinesFrame cm:SourceFrame .</t>
+  </si>
+  <si>
+    <t>StatementMap hasFrame CombinedFrame ;
+ResourceMap hasEvaluableExpression FunctionExpression ;
+FunctionExpression hasInput ExpressionList ;
+ExpressionList first DataField ;
+DataField belongsToFrame SourceFrame ;
+CombinedFrame combinesFrame SourceFrame ;</t>
+  </si>
+  <si>
+    <t>StatementMap hasFrame CombinedFrame ;
+ResourceMap hasEvaluableExpression FunctionExpression ;
+FunctionExpression hasInput ExpressionList ;
+ExpressionList first DataField ;
+DataField belongsToFrame SourceFrame ;
+SourceFrame hasNestedFrame SourceFrame ;</t>
+  </si>
+  <si>
+    <t>ResourceMap hasEvaluableExpression FunctionExpression ; 
+FunctionExpression hasFunctionName Concept ;</t>
+  </si>
+  <si>
+    <t>StatementMap SubClassOf hasSubject only NodeMap ;
+ReferenceNodeMap SubClassOf NodeMap ;
+BlankNodeMap SubClassOf NodeMap ;</t>
+  </si>
+  <si>
+    <t>StatementMap SubClassOf hasPredicate only ReferenceNodeMap ;</t>
+  </si>
+  <si>
+    <t>StatementMap SubClassOf hasObject only ResourceMap ;
+ReferenceNodeMap SubClassOf NodeMap ;
+BlankNodeMap SubClassOf NodeMap ;
+NodeMap SubClassOf ResourceMap ;
+LiteralMap SubClassOf ResourceMap ;
+LiteralMap SubClassOf ResourceMap ;
+ContainerMap SubClassOf ResourceMap ;</t>
+  </si>
+  <si>
+    <t>StatementMap SubClassOf hasNamedGraph only NodeMap ;
+ReferenceNodeMap SubClassOf NodeMap ;
+BlankNodeMap SubClassOf NodeMap ;</t>
+  </si>
+  <si>
+    <t>StatementMap hasDataType ListMap ;
+StatementMap hasDataType ReferenceNodeMap ;</t>
+  </si>
+  <si>
+    <t>StatementMap hasLanguage ListMap ;
+StatementMap hasLanguage LiteralMap ;</t>
+  </si>
+  <si>
+    <t>A datatype tag can only be expressed as an IRI or a List</t>
+  </si>
+  <si>
+    <t>A language tag can only be expressed as a Literal or a List</t>
+  </si>
+  <si>
+    <t>cm:StatementMap cm:hasDatatype cm:ReferenceNodeMap, cm:ListMap .</t>
+  </si>
+  <si>
+    <t>cm:StatementMap cm:hasLanguage cm:LiteralMap, cm:ListMap .</t>
+  </si>
+  <si>
+    <t>ConditionalStatementMap SubClassOf StatementMap ;
+ConditionalStatementMap hasBooleanCondition FunctionExpression ;</t>
+  </si>
+  <si>
+    <t>LinkingMap source StatementMap ;
+LinkingMap target StatementMap ;
+LinkingMap hasBooleanCondition FunctionExpression ;</t>
+  </si>
+  <si>
+    <t>cm:LinkingMap cm:hasBooleanCondition cm:FunctionExpression .
+cm:FunctionExpression hasFunctionName skos:Concept .</t>
+  </si>
+  <si>
+    <t>LinkingMap hasBooleanCondition FunctionExpression ;
+FunctionExpression hasFunctionName Concept ;</t>
+  </si>
+  <si>
+    <t>ResourceMap hasEvaluableExpression FunctionExpression ;
+FunctionExpression hasInput ExpressionList ;
+ExpressionList first FunctionExpression ;
+ExpressionList rest ExpressionList ;</t>
+  </si>
+  <si>
+    <t>SourceFrame hasNestedFrame SourceFrame ;</t>
+  </si>
+  <si>
+    <t>cm:SourceFrame cm:hasNestedFrame cm:SourceFrame .</t>
+  </si>
+  <si>
+    <t>cm:StatementMap cm:hasFrame cm:CombinedFrame ;
+    cm:hasObject cm:LiteralMap .
+cm:CombinedFrame cm:combinesFrame cm:SourceFrame, cm:CombinedFrame .
+cm:SourceFrame cm:hasDataSource cm:DataSource .</t>
+  </si>
+  <si>
+    <t>StatementMap hasObject LiteralMap ;
+StatementMap hasFrame CombinedFrame ;
+CombinedFrame combinesFrame SourceFrame ;
+CombinedFrame combinesFrame CombinedFrame ;
+SourceFrame hasDataSource DataSource ;</t>
+  </si>
+  <si>
+    <t>StatementMap hasDataType LiteralMap ;
+StatementMap hasLanguage LiteralMap ;
+StatementMap hasFrame CombinedFrame ;
+CombinedFrame combinesFrame SourceFrame ;
+CombinedFrame combinesFrame CombinedFrame ;
+SourceFrame hasDataSource DataSource ;</t>
   </si>
 </sst>
 </file>
@@ -429,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -470,6 +634,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,9 +923,9 @@
   </sheetPr>
   <dimension ref="A1:D1041"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -777,10 +944,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42">
@@ -791,7 +958,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>10</v>
@@ -802,10 +969,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>10</v>
@@ -816,10 +983,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14">
@@ -830,7 +997,7 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>10</v>
@@ -844,7 +1011,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
@@ -858,21 +1025,21 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" customHeight="1">
+    <row r="8" spans="1:4" ht="28">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>10</v>
@@ -883,80 +1050,80 @@
         <v>9</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56">
+    <row r="10" spans="1:4" ht="70">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14">
+    <row r="11" spans="1:4" ht="28">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="83" customHeight="1">
+    <row r="12" spans="1:4" ht="84">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="81" customHeight="1">
+    <row r="13" spans="1:4" ht="84">
       <c r="A13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="55" customHeight="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="84">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>10</v>
@@ -967,13 +1134,13 @@
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28">
@@ -981,24 +1148,24 @@
         <v>17</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" customHeight="1">
+    <row r="17" spans="1:4" ht="28">
       <c r="A17" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>10</v>
@@ -1009,10 +1176,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>10</v>
@@ -1023,13 +1190,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28">
@@ -1037,38 +1204,38 @@
         <v>21</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14">
+    <row r="21" spans="1:4" ht="28">
       <c r="A21" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
+    <row r="22" spans="1:4" ht="28">
       <c r="A22" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>10</v>
@@ -1079,38 +1246,38 @@
         <v>24</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="44" customHeight="1">
+    <row r="24" spans="1:4" ht="42">
       <c r="A24" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="42">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28">
       <c r="A25" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>10</v>
@@ -1118,58 +1285,58 @@
     </row>
     <row r="26" spans="1:4" ht="56">
       <c r="A26" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="56">
+    <row r="27" spans="1:4" ht="28">
       <c r="A27" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="70">
       <c r="A28" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="84">
       <c r="A29" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13"/>
@@ -5238,4 +5405,364 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A5B698-06C0-3B4E-8685-AE411587CE5F}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" ht="42">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28">
+      <c r="A4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28">
+      <c r="A5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="42">
+      <c r="A6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:4" ht="28">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="42">
+      <c r="A8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="168">
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:4" ht="84">
+      <c r="A10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="28">
+      <c r="A11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="126">
+      <c r="A12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="14"/>
+    </row>
+    <row r="13" spans="1:4" ht="182">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:4" ht="98">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="14"/>
+    </row>
+    <row r="15" spans="1:4" ht="98">
+      <c r="A15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:4" ht="42">
+      <c r="A16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="1:4" ht="56">
+      <c r="A17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" ht="28">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="112">
+      <c r="A19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" ht="56">
+      <c r="A20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" ht="28">
+      <c r="A21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28">
+      <c r="A22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="14"/>
+    </row>
+    <row r="23" spans="1:4" ht="56">
+      <c r="A23" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" ht="56">
+      <c r="A24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="1:4" ht="42">
+      <c r="A25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" ht="70">
+      <c r="A26" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" s="14"/>
+    </row>
+    <row r="27" spans="1:4" ht="28">
+      <c r="A27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" ht="70">
+      <c r="A28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" ht="84">
+      <c r="A29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
themis tests in new spreadsheet
</commit_message>
<xml_diff>
--- a/requirements/Requirements - conceptual mapping.xlsx
+++ b/requirements/Requirements - conceptual mapping.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiglesias/Documents/Conceptual-Mapping/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9006F0-7601-B94D-A793-DB6242A7868F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A62B74-0BE3-7946-9B4C-ECAFF4A01DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="500" windowWidth="26940" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="500" windowWidth="26940" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="Themis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
   <si>
     <t>Identifier</t>
   </si>
@@ -328,39 +327,6 @@
     <t>cm:DataSource cm:encoding xsd:string .</t>
   </si>
   <si>
-    <t>Themis test</t>
-  </si>
-  <si>
-    <t>SynchronousSource subclassof DataSource ;
-AsynchronousSource subclassof DataSource ;
-StreamSource subclassof DataSource ;</t>
-  </si>
-  <si>
-    <t>DataAccessService SubClassOf hasProtocol max 1 Concept ;</t>
-  </si>
-  <si>
-    <t>encoding domain DataSource ;</t>
-  </si>
-  <si>
-    <t>DataSource mediaType MediaType ;</t>
-  </si>
-  <si>
-    <t>DataAccessService hasSecurityScheme SecurityScheme ;</t>
-  </si>
-  <si>
-    <t>DataSource accessService DataAccessService ;</t>
-  </si>
-  <si>
-    <t>DataService servesDataset Dataset ;</t>
-  </si>
-  <si>
-    <t>StatementMap hasFrame CombinedFrame ;
-CombinedFrame SubClassOf combinesFrame exactly 2 Frame ;
-SourceFrame SubClassOf Frame ;
-SourceFrame hasDataSource DataSource ;
-SourceFrame hasNestedFrame SourceFrame ;</t>
-  </si>
-  <si>
     <t>cm:StatementMap cm:hasFrame cm:CombinedFrame .
 cm:CombinedFrame cm:combinesFrame cm:SourceFrame, cm:CombinedFrame .
 cm:SourceFrame cm:hasDataSource cm:DataSource ;
@@ -368,38 +334,6 @@
   </si>
   <si>
     <t>A source frame describes exactly one data source</t>
-  </si>
-  <si>
-    <t>SourceFrame SubClassOf hasDataSource exactly 1 DataSource ;</t>
-  </si>
-  <si>
-    <t>StatementMap hasSubject NodeMap ;
-StatementMap hasPredicate ReferenceNodeMap ;
-StatementMap hasObject ResourceMap ;
-ReferenceNodeMap SubClassOf NodeMap ;
-NodeMap SubClassOf ResourceMap ;
-ResourceMap hasEvaluableExpression EvaluableExpression ;
-Constant SubClassOf EvaluableExpression ;
-DataField SubClassOf EvaluableExpression ;</t>
-  </si>
-  <si>
-    <t>StatementMap SubClassOf hasSubject exactly 1 NodeMap ;
-StatementMap SubClassOf hasPredicate exactly 1 ReferenceNodeMap ;
-StatementMap SubClassOf hasObject exactly 1 ResourceMap ;
-StatementMap SubClassOf hasNamedGraph max 1 NodeMap ;
-StatementMap SubClassOf hasDataType max 1 ReferenceNodeMap ;
-StatementMap SubClassOf hasLanguage max 1 LiteralMap ;</t>
-  </si>
-  <si>
-    <t>StatementMap SubClassOf hasNamedGraph max 1 NodeMap ;
-StatementMap SubClassOf hasDataType max 1 ReferenceNodeMap ;
-StatementMap SubClassOf hasLanguage max 1 LiteralMap ;
-ReferenceNodeMap SubClassOf NodeMap ;
-NodeMap SubClassOf ResourceMap ;
-LiteralMap SubClassOf ResourceMap ;
-ResourceMap hasEvaluableExpression EvaluableExpression ;
-Constant SubClassOf EvaluableExpression ;
-DataField SubClassOf EvaluableExpression ;</t>
   </si>
   <si>
     <t>cm:StatementMap cm:hasFrame cm:CombinedFrame .
@@ -410,56 +344,6 @@
 cm:CombinedFrame cm:combinesFrame cm:SourceFrame .</t>
   </si>
   <si>
-    <t>StatementMap hasFrame CombinedFrame ;
-ResourceMap hasEvaluableExpression FunctionExpression ;
-FunctionExpression hasInput ExpressionList ;
-ExpressionList first DataField ;
-DataField belongsToFrame SourceFrame ;
-CombinedFrame combinesFrame SourceFrame ;</t>
-  </si>
-  <si>
-    <t>StatementMap hasFrame CombinedFrame ;
-ResourceMap hasEvaluableExpression FunctionExpression ;
-FunctionExpression hasInput ExpressionList ;
-ExpressionList first DataField ;
-DataField belongsToFrame SourceFrame ;
-SourceFrame hasNestedFrame SourceFrame ;</t>
-  </si>
-  <si>
-    <t>ResourceMap hasEvaluableExpression FunctionExpression ; 
-FunctionExpression hasFunctionName Concept ;</t>
-  </si>
-  <si>
-    <t>StatementMap SubClassOf hasSubject only NodeMap ;
-ReferenceNodeMap SubClassOf NodeMap ;
-BlankNodeMap SubClassOf NodeMap ;</t>
-  </si>
-  <si>
-    <t>StatementMap SubClassOf hasPredicate only ReferenceNodeMap ;</t>
-  </si>
-  <si>
-    <t>StatementMap SubClassOf hasObject only ResourceMap ;
-ReferenceNodeMap SubClassOf NodeMap ;
-BlankNodeMap SubClassOf NodeMap ;
-NodeMap SubClassOf ResourceMap ;
-LiteralMap SubClassOf ResourceMap ;
-LiteralMap SubClassOf ResourceMap ;
-ContainerMap SubClassOf ResourceMap ;</t>
-  </si>
-  <si>
-    <t>StatementMap SubClassOf hasNamedGraph only NodeMap ;
-ReferenceNodeMap SubClassOf NodeMap ;
-BlankNodeMap SubClassOf NodeMap ;</t>
-  </si>
-  <si>
-    <t>StatementMap hasDataType ListMap ;
-StatementMap hasDataType ReferenceNodeMap ;</t>
-  </si>
-  <si>
-    <t>StatementMap hasLanguage ListMap ;
-StatementMap hasLanguage LiteralMap ;</t>
-  </si>
-  <si>
     <t>A datatype tag can only be expressed as an IRI or a List</t>
   </si>
   <si>
@@ -470,32 +354,10 @@
   </si>
   <si>
     <t>cm:StatementMap cm:hasLanguage cm:LiteralMap, cm:ListMap .</t>
-  </si>
-  <si>
-    <t>ConditionalStatementMap SubClassOf StatementMap ;
-ConditionalStatementMap hasBooleanCondition FunctionExpression ;</t>
-  </si>
-  <si>
-    <t>LinkingMap source StatementMap ;
-LinkingMap target StatementMap ;
-LinkingMap hasBooleanCondition FunctionExpression ;</t>
   </si>
   <si>
     <t>cm:LinkingMap cm:hasBooleanCondition cm:FunctionExpression .
 cm:FunctionExpression hasFunctionName skos:Concept .</t>
-  </si>
-  <si>
-    <t>LinkingMap hasBooleanCondition FunctionExpression ;
-FunctionExpression hasFunctionName Concept ;</t>
-  </si>
-  <si>
-    <t>ResourceMap hasEvaluableExpression FunctionExpression ;
-FunctionExpression hasInput ExpressionList ;
-ExpressionList first FunctionExpression ;
-ExpressionList rest ExpressionList ;</t>
-  </si>
-  <si>
-    <t>SourceFrame hasNestedFrame SourceFrame ;</t>
   </si>
   <si>
     <t>cm:SourceFrame cm:hasNestedFrame cm:SourceFrame .</t>
@@ -505,21 +367,6 @@
     cm:hasObject cm:LiteralMap .
 cm:CombinedFrame cm:combinesFrame cm:SourceFrame, cm:CombinedFrame .
 cm:SourceFrame cm:hasDataSource cm:DataSource .</t>
-  </si>
-  <si>
-    <t>StatementMap hasObject LiteralMap ;
-StatementMap hasFrame CombinedFrame ;
-CombinedFrame combinesFrame SourceFrame ;
-CombinedFrame combinesFrame CombinedFrame ;
-SourceFrame hasDataSource DataSource ;</t>
-  </si>
-  <si>
-    <t>StatementMap hasDataType LiteralMap ;
-StatementMap hasLanguage LiteralMap ;
-StatementMap hasFrame CombinedFrame ;
-CombinedFrame combinesFrame SourceFrame ;
-CombinedFrame combinesFrame CombinedFrame ;
-SourceFrame hasDataSource DataSource ;</t>
   </si>
 </sst>
 </file>
@@ -593,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -634,9 +481,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -923,7 +767,7 @@
   </sheetPr>
   <dimension ref="A1:D1041"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
@@ -1067,7 +911,7 @@
         <v>55</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>10</v>
@@ -1078,7 +922,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
@@ -1123,7 +967,7 @@
         <v>56</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>10</v>
@@ -1218,10 +1062,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>10</v>
@@ -1232,10 +1076,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>10</v>
@@ -1277,7 +1121,7 @@
         <v>46</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>10</v>
@@ -1305,7 +1149,7 @@
         <v>48</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>49</v>
@@ -1319,7 +1163,7 @@
         <v>59</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>50</v>
@@ -5405,364 +5249,4 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A5B698-06C0-3B4E-8685-AE411587CE5F}">
-  <dimension ref="A1:D29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="57.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="42">
-      <c r="A2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:4" ht="42">
-      <c r="A3" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28">
-      <c r="A4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28">
-      <c r="A5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="42">
-      <c r="A6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="1:4" ht="28">
-      <c r="A7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="42">
-      <c r="A8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="168">
-      <c r="A9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:4" ht="84">
-      <c r="A10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" ht="28">
-      <c r="A11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="126">
-      <c r="A12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="1:4" ht="182">
-      <c r="A13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:4" ht="98">
-      <c r="A14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:4" ht="98">
-      <c r="A15" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:4" ht="42">
-      <c r="A16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4" ht="56">
-      <c r="A17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" ht="28">
-      <c r="A18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="112">
-      <c r="A19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" ht="56">
-      <c r="A20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="1:4" ht="28">
-      <c r="A21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28">
-      <c r="A22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="14"/>
-    </row>
-    <row r="23" spans="1:4" ht="56">
-      <c r="A23" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" ht="56">
-      <c r="A24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:4" ht="42">
-      <c r="A25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="1:4" ht="70">
-      <c r="A26" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:4" ht="28">
-      <c r="A27" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="10"/>
-    </row>
-    <row r="28" spans="1:4" ht="70">
-      <c r="A28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="1:4" ht="84">
-      <c r="A29" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D29" s="10"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>